<commit_message>
Add demographics analysis to the assembled 1-7 chapter ipynb file.
</commit_message>
<xml_diff>
--- a/HeroesOfPymoli/5_Top_Spenders.xlsx
+++ b/HeroesOfPymoli/5_Top_Spenders.xlsx
@@ -451,7 +451,7 @@
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>Chamjask73</t>
+          <t>Hiaral50</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -459,19 +459,19 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>$4.61</t>
+          <t>$1.40</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>$13.83</t>
+          <t>$4.19</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>Rarallo90</t>
+          <t>Raesty92</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -479,12 +479,12 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>$3.02</t>
+          <t>$2.91</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>$9.05</t>
+          <t>$8.73</t>
         </is>
       </c>
     </row>

</xml_diff>